<commit_message>
Update example.xlsx Added extra sheets
</commit_message>
<xml_diff>
--- a/books/AutomateTheBoringStuffWithPython/Chapter12/example.xlsx
+++ b/books/AutomateTheBoringStuffWithPython/Chapter12/example.xlsx
@@ -9,6 +9,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -53,6 +55,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -146,8 +149,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="21.9489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -236,4 +239,56 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>